<commit_message>
Update maps/BloodVolumeControlv1.xlsx with component and flatmap id columns.
</commit_message>
<xml_diff>
--- a/maps/BloodVolumeControlv1.xlsx
+++ b/maps/BloodVolumeControlv1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/phun025_uoa_auckland_ac_nz/Documents/Documents/BG lectures/BG 6. FPUs/ANS-CVS model for REVEAL/Blood volume control v1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/biotechtwin/fc-feature-mapping/maps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="8_{A0B8095D-AEFC-4245-AA0C-228ACE32BD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17E6B6C2-53FF-415A-9AE1-0BBCDEDE28B4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{094BE5F9-B325-B141-BD3E-445266AD8BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="180" windowWidth="22050" windowHeight="15250" xr2:uid="{A1727B0C-5977-4211-B036-5140AE803B9C}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="21680" xr2:uid="{A1727B0C-5977-4211-B036-5140AE803B9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -506,13 +506,97 @@
   </si>
   <si>
     <t>Flux of water through epithelial cell of proximal tubule</t>
+  </si>
+  <si>
+    <t>Flatmap ID</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000040</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000041</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000023</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000043</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000021</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000019</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000066</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000059</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000067</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000017</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000038</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000010</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000011</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000012</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000009</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000033</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000029</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000028</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000036</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000050</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000032</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000064</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000053</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000031</t>
+  </si>
+  <si>
+    <t>bvc/ID-0000065</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>main</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -545,6 +629,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -589,7 +680,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -606,6 +697,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -624,10 +716,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1131,22 +1219,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3512D18F-6A89-4572-BF93-3D5D9EC1DDE3}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" customWidth="1"/>
-    <col min="2" max="2" width="7.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.90625" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1157,22 +1245,30 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G1" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="6"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1182,14 +1278,20 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="5" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1199,11 +1301,17 @@
       <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G4" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1213,14 +1321,17 @@
       <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="5" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="5" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1230,14 +1341,20 @@
       <c r="C6" s="5">
         <v>0.84</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="5" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1247,14 +1364,20 @@
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="5" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="5" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1264,23 +1387,31 @@
       <c r="C8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="5" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="5" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="6"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1290,14 +1421,20 @@
       <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="5" t="e" vm="6">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="5" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1307,14 +1444,20 @@
       <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="5" t="e" vm="7">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="5" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -1324,14 +1467,20 @@
       <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="5" t="e" vm="8">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="5" t="e" vm="8">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1341,14 +1490,20 @@
       <c r="C13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="5" t="e" vm="9">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="5" t="e" vm="9">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1358,11 +1513,17 @@
       <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G14" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1372,14 +1533,20 @@
       <c r="C15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="5" t="e" vm="10">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="5" t="e" vm="10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1389,14 +1556,20 @@
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="5" t="e" vm="11">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="5" t="e" vm="11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1406,14 +1579,20 @@
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="5" t="e" vm="12">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="5" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -1423,14 +1602,20 @@
       <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="5" t="e" vm="13">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="5" t="e" vm="13">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1440,14 +1625,20 @@
       <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="5" t="e" vm="14">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="5" t="e" vm="14">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1457,23 +1648,31 @@
       <c r="C20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="5" t="e" vm="15">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="5" t="e" vm="15">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D21" s="7"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1483,14 +1682,20 @@
       <c r="C22" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="5" t="e" vm="16">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="5" t="e" vm="16">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1500,14 +1705,20 @@
       <c r="C23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="5" t="e" vm="17">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="5" t="e" vm="17">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1517,14 +1728,20 @@
       <c r="C24" s="5">
         <v>0.01</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="5" t="e" vm="18">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="5" t="e" vm="18">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1534,25 +1751,37 @@
       <c r="C25" s="5">
         <v>0.1</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="5" t="e" vm="19">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="5" t="e" vm="19">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1562,14 +1791,20 @@
       <c r="C27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="5" t="e" vm="20">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="5" t="e" vm="20">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1579,14 +1814,20 @@
       <c r="C28" s="5">
         <v>1.2E-2</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="5" t="e" vm="21">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="5" t="e" vm="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1596,14 +1837,20 @@
       <c r="C29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="5" t="e" vm="22">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="5" t="e" vm="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1613,14 +1860,20 @@
       <c r="C30" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="5" t="e" vm="23">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="5" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1630,14 +1883,20 @@
       <c r="C31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="5" t="e" vm="24">
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="5" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1647,11 +1906,17 @@
       <c r="C32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" t="s">
         <v>59</v>
       </c>
-      <c r="E32" s="5" t="e" vm="25">
-        <v>#VALUE!</v>
+      <c r="F32" s="5" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G32" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>